<commit_message>
Finalizando exploração dos dados + Excel finalizado
</commit_message>
<xml_diff>
--- a/Organizando dados.xlsx
+++ b/Organizando dados.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projetos\Projeto-Analise-de-Dados-SRAG-2021---2024-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEED2F8E-D6C3-4229-87F2-DA79CF5D97DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C430A57-9F60-4123-9E69-C0CC48E33608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{ED5AD74C-555A-40DA-A62E-D3459C7593AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED5AD74C-555A-40DA-A62E-D3459C7593AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionário de dados" sheetId="1" r:id="rId1"/>
     <sheet name="Colunas 2021" sheetId="2" r:id="rId2"/>
     <sheet name="Colunas 2022" sheetId="3" r:id="rId3"/>
+    <sheet name="Colunas 2023" sheetId="4" r:id="rId4"/>
+    <sheet name="Colunas 2024" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="434">
   <si>
     <t>Colunas</t>
   </si>
@@ -1520,7 +1522,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="20">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1590,14 +1610,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15A3C35E-69DB-49C3-8782-A477CA4F7916}" name="Tabela2" displayName="Tabela2" ref="A1:E180" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15A3C35E-69DB-49C3-8782-A477CA4F7916}" name="Tabela2" displayName="Tabela2" ref="A1:E180" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="A1:E180" xr:uid="{15A3C35E-69DB-49C3-8782-A477CA4F7916}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1CF15E86-3FDE-4FFA-9334-2AEBB16457FE}" name="Colunas" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{0CEBB635-FD59-43DF-B13A-7590569F95EA}" name="Descrição" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{7AA778D0-3214-431F-8677-07FA74A3315A}" name="Colunas que serao desconsideradas" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{519AB8D9-E9F1-42C7-99BD-27E35607C102}" name="Comentarios" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{09C524F9-C1AA-4C82-8E7C-4791DD8BBFB7}" name="Porque sera desconsiderada" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{1CF15E86-3FDE-4FFA-9334-2AEBB16457FE}" name="Colunas" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{0CEBB635-FD59-43DF-B13A-7590569F95EA}" name="Descrição" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{7AA778D0-3214-431F-8677-07FA74A3315A}" name="Colunas que serao desconsideradas" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{519AB8D9-E9F1-42C7-99BD-27E35607C102}" name="Comentarios" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{09C524F9-C1AA-4C82-8E7C-4791DD8BBFB7}" name="Porque sera desconsiderada" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1607,11 +1627,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F0710EE-F857-4ED5-AD97-1D4A264D9A60}" name="Tabela1" displayName="Tabela1" ref="A1:C120" totalsRowShown="0">
   <autoFilter ref="A1:C120" xr:uid="{3F0710EE-F857-4ED5-AD97-1D4A264D9A60}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C689C462-CF9A-4A49-9651-2D11B10EBFDA}" name="Coluna" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{17816C4B-1900-4889-B6B8-D193E59A1621}" name="Descrição" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{C689C462-CF9A-4A49-9651-2D11B10EBFDA}" name="Coluna" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{17816C4B-1900-4889-B6B8-D193E59A1621}" name="Descrição" dataDxfId="10">
       <calculatedColumnFormula>VLOOKUP(A2,Tabela2[#All], 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAFED104-51D5-4C6B-AEE2-A7443C1CD690}" name="Comentarios" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{BAFED104-51D5-4C6B-AEE2-A7443C1CD690}" name="Comentarios" dataDxfId="9">
       <calculatedColumnFormula>VLOOKUP(A2,Tabela2[#All], 4, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1623,12 +1643,42 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{22DCAE45-34F3-43DA-ABB2-A390DE9C0B09}" name="Tabela5" displayName="Tabela5" ref="A1:C125" totalsRowShown="0">
   <autoFilter ref="A1:C125" xr:uid="{22DCAE45-34F3-43DA-ABB2-A390DE9C0B09}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C12E8AFF-7332-431B-B8AB-E18936ED34F4}" name="Coluna" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{C5A45C42-4987-4EBE-8150-FAD68D1402CA}" name="Descrição" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{C12E8AFF-7332-431B-B8AB-E18936ED34F4}" name="Coluna" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{C5A45C42-4987-4EBE-8150-FAD68D1402CA}" name="Descrição" dataDxfId="7">
       <calculatedColumnFormula>VLOOKUP(A2,Tabela2[#All], 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AFDD444F-E3D6-46B1-A5BB-F2EB0B5AA68A}" name="Comentarios" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{AFDD444F-E3D6-46B1-A5BB-F2EB0B5AA68A}" name="Comentarios" dataDxfId="6">
       <calculatedColumnFormula>VLOOKUP(A2,Tabela2[#All], 4, FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9CDAEF83-3897-421C-B19E-79F681C89CAB}" name="Tabela6" displayName="Tabela6" ref="A1:C125" totalsRowShown="0">
+  <autoFilter ref="A1:C125" xr:uid="{9CDAEF83-3897-421C-B19E-79F681C89CAB}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6E824EEE-4D3E-4A4C-ACD4-C34FDF2222D5}" name="Coluna" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8AAE18F0-819B-4B63-8472-85486D0525E0}" name="Descrição" dataDxfId="4">
+      <calculatedColumnFormula>VLOOKUP(A2,Tabela5[#All], 2, FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{9FD068A1-84AC-4310-AB9F-BC9543236C1A}" name="Comentarios" dataDxfId="3">
+      <calculatedColumnFormula>VLOOKUP(A2,Tabela5[#All], 3, FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{561FAB62-AB79-4AB3-8EEC-365C678C2793}" name="Tabela7" displayName="Tabela7" ref="A1:C125" totalsRowShown="0">
+  <autoFilter ref="A1:C125" xr:uid="{561FAB62-AB79-4AB3-8EEC-365C678C2793}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{29DDBFA6-7126-42C5-9764-54F2BDC4C510}" name="Coluna" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{14196F86-282F-4B24-A4A8-A40447E3C3AD}" name="Descrição" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{236846AE-49F3-497C-846E-1659994C4E5A}" name="Comentarios" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP(A2,Tabela6[#All], 3, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1954,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831FF6EA-A12F-46F3-B86A-ED578ABDB804}">
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E180"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5040,8 +5090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFEC88C-6AFE-43DD-B607-144D5438B390}">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C120"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6738,8 +6788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF9289B-A554-48A1-A389-CBF5BD58907C}">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8498,6 +8548,3556 @@
       </c>
       <c r="C125" s="1" t="str">
         <f>VLOOKUP(A125,Tabela2[#All], 4, FALSE)</f>
+        <v>1-Nirmatrevir/ritonavir(Paxlovid ®)
+2- Molnupiravir(Lagevrio®)
+3- Baricitinibe (Olumiant®)
+4- Outro, especifique</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3D6F48-7B87-431C-9BFE-39E88310097E}">
+  <dimension ref="A1:C125"/>
+  <sheetViews>
+    <sheetView topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>VLOOKUP(A2,Tabela5[#All], 2, FALSE)</f>
+        <v>Semana Epidemiológica do preenchimento da ficha de notificação</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>VLOOKUP(A2,Tabela5[#All], 3, FALSE)</f>
+        <v>As Semanas Epidemiológicas (SE) são contadas de um Domingo até o Sábado.
+Se o ano começa em uma segunda-feira, a 1ª SE começará no domingo da mesma semana.</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>VLOOKUP(A3,Tabela5[#All], 2, FALSE)</f>
+        <v>Semana Epidemiológica do início dos sintomas</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>VLOOKUP(A3,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>VLOOKUP(A4,Tabela5[#All], 2, FALSE)</f>
+        <v>Unidade Federativa</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>VLOOKUP(A4,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f>VLOOKUP(A5,Tabela5[#All], 2, FALSE)</f>
+        <v>Regional de Saúde</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f>VLOOKUP(A6,Tabela5[#All], 2, FALSE)</f>
+        <v>Município</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f>VLOOKUP(A7,Tabela5[#All], 2, FALSE)</f>
+        <v>Unidade que realizou o atendimento, coleta de amostra e registro do caso</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f>VLOOKUP(A8,Tabela5[#All], 2, FALSE)</f>
+        <v>Sexo do paciente</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f>VLOOKUP(A8,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Masculino
+2-Feminino
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>VLOOKUP(A9,Tabela5[#All], 2, FALSE)</f>
+        <v>Idade do paciente</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>VLOOKUP(A9,Tabela5[#All], 3, FALSE)</f>
+        <v>Caso tenha sido fornecida a data de nascimento esse campo é preenchido automaticamente (considerando o intervalo entre a data de nascimento e a data dos primeiros sintomas), caso não, é preenchido com a idade informada pelo paciente</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f>VLOOKUP(A10,Tabela5[#All], 2, FALSE)</f>
+        <v>Tipo do campo idade</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>VLOOKUP(A10,Tabela5[#All], 3, FALSE)</f>
+        <v>Se a diferença entre a data de nascimento e a data dos primeiros sintomas for:
+Menor que 1 mês: o tipo é preenchido como 1-Dia
+De 1 a 11 meses: o tipo é preenchido como 2-Mês
+Maior ou igual a 12 meses: o tipo é preenchido como 3-Ano</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>VLOOKUP(A11,Tabela5[#All], 2, FALSE)</f>
+        <v xml:space="preserve">Idade gestacional da paciente.
+</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>VLOOKUP(A11,Tabela5[#All], 3, FALSE)</f>
+        <v>1-1º Trimestre
+2-2º Trimestre
+3-3º Trimestre
+4-Idade Gestacional Ignorada
+5-Não
+6-Não se aplica
+9-Ignorado
+Se selecionado sexo igual a Masculino ou a idade for menor ou igual a 9 anos o campo é preenchido automaticamente com 6-Não se aplica</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f>VLOOKUP(A12,Tabela5[#All], 2, FALSE)</f>
+        <v>Cor ou raça declarada pelo paciente</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>VLOOKUP(A12,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Branca
+2-Preta
+3-Amarela
+4-Parda
+5-Indígena
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f>VLOOKUP(A13,Tabela5[#All], 2, FALSE)</f>
+        <v>Nível de escolaridade do paciente</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>VLOOKUP(A13,Tabela5[#All], 3, FALSE)</f>
+        <v>0-Sem escolaridade/ Analfabeto
+1-Fundamental 1º ciclo (1ª a 5ª série)
+2-Fundamental 2º ciclo (6ª a 9ª série)
+3- Médio (1º ao 3º ano)
+4-Superior
+5-Não se aplica
+9-Ignorado
+Se o paciente tiver menos de 7 anos é automaticamente preenchido com a categoria “não se aplica”</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f>VLOOKUP(A14,Tabela5[#All], 2, FALSE)</f>
+        <v>País de residência do paciente</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f>VLOOKUP(A15,Tabela5[#All], 2, FALSE)</f>
+        <v>UF da residência</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f>VLOOKUP(A16,Tabela5[#All], 2, FALSE)</f>
+        <v>Regional de Saúde onde está localizado o Município de residência do paciente</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f>VLOOKUP(A17,Tabela5[#All], 2, FALSE)</f>
+        <v>Município de residência do paciente</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f>VLOOKUP(A18,Tabela5[#All], 2, FALSE)</f>
+        <v>Zona geográfica da residência</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>VLOOKUP(A18,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Urbana
+2-Rural
+3-Periurbana
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f>VLOOKUP(A19,Tabela5[#All], 2, FALSE)</f>
+        <v>Caso de SRAG com infecção adquirida após internação</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f>VLOOKUP(A19,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f>VLOOKUP(A20,Tabela5[#All], 2, FALSE)</f>
+        <v>Caso com contato direto com aves ou suínos</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>VLOOKUP(A20,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f>VLOOKUP(A21,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou febre</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>VLOOKUP(A21,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f>VLOOKUP(A22,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou tosse</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f>VLOOKUP(A22,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f>VLOOKUP(A23,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou dor de garganta</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f>VLOOKUP(A23,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f>VLOOKUP(A24,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou dispneia</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f>VLOOKUP(A24,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f>VLOOKUP(A25,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou desconforto respiratório</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>VLOOKUP(A25,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f>VLOOKUP(A26,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou saturção O2 &lt; 95%</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f>VLOOKUP(A26,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f>VLOOKUP(A27,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou diarreia</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f>VLOOKUP(A27,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f>VLOOKUP(A28,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou vômito</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <f>VLOOKUP(A28,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <f>VLOOKUP(A29,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou outros sintomas</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <f>VLOOKUP(A29,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <f>VLOOKUP(A30,Tabela5[#All], 2, FALSE)</f>
+        <v>Lista outros sintomas</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <f>VLOOKUP(A30,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <f>VLOOKUP(A31,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente é puérpera ou parturiente (até 45 dias após o parto)</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <f>VLOOKUP(A31,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <f>VLOOKUP(A32,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresenta algum fator de risco</v>
+      </c>
+      <c r="C32" s="1" t="str">
+        <f>VLOOKUP(A32,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <f>VLOOKUP(A33,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui doença cardiovascular crônica</v>
+      </c>
+      <c r="C33" s="1" t="str">
+        <f>VLOOKUP(A33,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <f>VLOOKUP(A34,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui doença hematológica crônica</v>
+      </c>
+      <c r="C34" s="1" t="str">
+        <f>VLOOKUP(A34,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f>VLOOKUP(A35,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui síndrome de down</v>
+      </c>
+      <c r="C35" s="1" t="str">
+        <f>VLOOKUP(A35,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f>VLOOKUP(A36,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui doença hepática crônica</v>
+      </c>
+      <c r="C36" s="1" t="str">
+        <f>VLOOKUP(A36,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f>VLOOKUP(A37,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui asma</v>
+      </c>
+      <c r="C37" s="1" t="str">
+        <f>VLOOKUP(A37,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f>VLOOKUP(A38,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui diabetes mellitus</v>
+      </c>
+      <c r="C38" s="1" t="str">
+        <f>VLOOKUP(A38,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f>VLOOKUP(A39,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui doença neurológica</v>
+      </c>
+      <c r="C39" s="1" t="str">
+        <f>VLOOKUP(A39,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f>VLOOKUP(A40,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui pneumopatia crônica</v>
+      </c>
+      <c r="C40" s="1" t="str">
+        <f>VLOOKUP(A40,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f>VLOOKUP(A41,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui imunodeficiência ou imunodpressão</v>
+      </c>
+      <c r="C41" s="1" t="str">
+        <f>VLOOKUP(A41,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="1" t="str">
+        <f>VLOOKUP(A42,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui doença renal crônica</v>
+      </c>
+      <c r="C42" s="1" t="str">
+        <f>VLOOKUP(A42,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" s="1" t="str">
+        <f>VLOOKUP(A43,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui obesidade</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <f>VLOOKUP(A43,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" s="1" t="str">
+        <f>VLOOKUP(A44,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente possui outro fator de risco</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <f>VLOOKUP(A44,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="1" t="str">
+        <f>VLOOKUP(A45,Tabela5[#All], 2, FALSE)</f>
+        <v>Lista outros fatores de risco do paciente</v>
+      </c>
+      <c r="C45" s="1" t="str">
+        <f>VLOOKUP(A45,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B46" s="1" t="str">
+        <f>VLOOKUP(A46,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente foi vacinado contra a gripe na última campanha</v>
+      </c>
+      <c r="C46" s="1" t="str">
+        <f>VLOOKUP(A46,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B47" s="1" t="str">
+        <f>VLOOKUP(A47,Tabela5[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver menos que 6 meses de vida, a mãe recebeu vacina</v>
+      </c>
+      <c r="C47" s="1" t="str">
+        <f>VLOOKUP(A47,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" s="1" t="str">
+        <f>VLOOKUP(A48,Tabela5[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver menos que 6 meses, a mãe amamenta a criança</v>
+      </c>
+      <c r="C48" s="1" t="str">
+        <f>VLOOKUP(A48,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B49" s="1" t="str">
+        <f>VLOOKUP(A49,Tabela5[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver entre 6 meses e 8 anos, data da dose única para crianças vacinadas em campanhas de anos anteriores</v>
+      </c>
+      <c r="C49" s="1" t="str">
+        <f>VLOOKUP(A49,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B50" s="1" t="str">
+        <f>VLOOKUP(A50,Tabela5[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver entre 6 meses e 8 anos, data da 1a dose para crianças vacinadas pela primeira vez</v>
+      </c>
+      <c r="C50" s="1" t="str">
+        <f>VLOOKUP(A50,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f>VLOOKUP(A51,Tabela5[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver entre 6 meses e 8 anos, data da 2a dose para crianças vacinadas pela primeira vez</v>
+      </c>
+      <c r="C51" s="1" t="str">
+        <f>VLOOKUP(A51,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f>VLOOKUP(A52,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente usou antiviral para gripe</v>
+      </c>
+      <c r="C52" s="1" t="str">
+        <f>VLOOKUP(A52,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f>VLOOKUP(A53,Tabela5[#All], 2, FALSE)</f>
+        <v>Qual antiviral</v>
+      </c>
+      <c r="C53" s="1" t="str">
+        <f>VLOOKUP(A53,Tabela5[#All], 3, FALSE)</f>
+        <v>1- Oseltamivir
+2- Zanamivir
+3- Outro, especifique</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f>VLOOKUP(A54,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente foi internado</v>
+      </c>
+      <c r="C54" s="1" t="str">
+        <f>VLOOKUP(A54,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f>VLOOKUP(A55,Tabela5[#All], 2, FALSE)</f>
+        <v>UF onde o paciente foi internado</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f>VLOOKUP(A56,Tabela5[#All], 2, FALSE)</f>
+        <v>Regional de Saúde onde o paciente foi internado</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f>VLOOKUP(A57,Tabela5[#All], 2, FALSE)</f>
+        <v>Município onde o paciente foi internado</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f>VLOOKUP(A58,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente foi internado na UTI</v>
+      </c>
+      <c r="C58" s="1" t="str">
+        <f>VLOOKUP(A58,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f>VLOOKUP(A59,Tabela5[#All], 2, FALSE)</f>
+        <v>Data de entrada na UTI</v>
+      </c>
+      <c r="C59" s="1" t="str">
+        <f>VLOOKUP(A59,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f>VLOOKUP(A60,Tabela5[#All], 2, FALSE)</f>
+        <v>Data de saída da UTI</v>
+      </c>
+      <c r="C60" s="1" t="str">
+        <f>VLOOKUP(A60,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f>VLOOKUP(A61,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente fez uso de suporte ventilatório</v>
+      </c>
+      <c r="C61" s="1" t="str">
+        <f>VLOOKUP(A61,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim, invasivo
+2-Sim, não invasivo
+3-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f>VLOOKUP(A62,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado Raio-X de tórax</v>
+      </c>
+      <c r="C62" s="1" t="str">
+        <f>VLOOKUP(A62,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Normal_x000D_
+2-Infiltrado intersticial_x000D_
+3-Consolidação_x000D_
+4-Misto_x000D_
+5-Outro_x000D_
+6-Não realizado_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B63" s="1" t="str">
+        <f>VLOOKUP(A63,Tabela5[#All], 2, FALSE)</f>
+        <v>Foi realizado coleta de amostra na realização do teste diagnóstico</v>
+      </c>
+      <c r="C63" s="1" t="str">
+        <f>VLOOKUP(A63,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B64" s="1" t="str">
+        <f>VLOOKUP(A64,Tabela5[#All], 2, FALSE)</f>
+        <v>Tipo da amostra</v>
+      </c>
+      <c r="C64" s="1" t="str">
+        <f>VLOOKUP(A64,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Secreção de Nasoorofaringe_x000D_
+2-Lavado Broco-alveolar_x000D_
+3-Tecido post-mortem_x000D_
+4-Outra, qual?_x000D_
+5-LCR_x000D_
+9-Ignorado_x000D_</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B65" s="1" t="str">
+        <f>VLOOKUP(A65,Tabela5[#All], 2, FALSE)</f>
+        <v>Se for colhida amostra, resultado do teste RT-PCR ou outro método</v>
+      </c>
+      <c r="C65" s="1" t="str">
+        <f>VLOOKUP(A65,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Detectável
+2-Não Detectável
+3-Inconclusivo
+4-Não Realizado
+5-Aguardando Resultado
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B66" s="1" t="str">
+        <f>VLOOKUP(A66,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do RT-PCR foi positivo para influenza</v>
+      </c>
+      <c r="C66" s="1" t="str">
+        <f>VLOOKUP(A66,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim_x000D_
+2-Não_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B67" s="1" t="str">
+        <f>VLOOKUP(A67,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do diagnóstico do RT-PCR para o tipo de influenza</v>
+      </c>
+      <c r="C67" s="1" t="str">
+        <f>VLOOKUP(A67,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Influenza A_x000D_
+2-Influenza B</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B68" s="1" t="str">
+        <f>VLOOKUP(A68,Tabela5[#All], 2, FALSE)</f>
+        <v>Subtipo para Influenza A</v>
+      </c>
+      <c r="C68" s="1" t="str">
+        <f>VLOOKUP(A68,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Influenza A(H1N1)pdm09_x000D_
+2-Influenza A (H3N2)_x000D_
+3-Influenza A não subtipado_x000D_
+4-Influenza A não subtipável_x000D_
+5-Inconclusivo_x000D_
+6-Outro, especifique</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B69" s="1" t="str">
+        <f>VLOOKUP(A69,Tabela5[#All], 2, FALSE)</f>
+        <v>Linhagem da Influenza B</v>
+      </c>
+      <c r="C69" s="1" t="str">
+        <f>VLOOKUP(A69,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Victoria
+2-Yamagatha
+3-Não realizado
+4-Inconclusivo
+5-Outro, especifique:</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <f>VLOOKUP(A70,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do RT-PCR foi positivo para outro vírus respiratório</v>
+      </c>
+      <c r="C70" s="1" t="str">
+        <f>VLOOKUP(A70,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B71" s="1" t="str">
+        <f>VLOOKUP(A71,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para VSR</v>
+      </c>
+      <c r="C71" s="1" t="str">
+        <f>VLOOKUP(A71,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="B72" s="1" t="str">
+        <f>VLOOKUP(A72,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Parainfluenza 1</v>
+      </c>
+      <c r="C72" s="1" t="str">
+        <f>VLOOKUP(A72,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B73" s="1" t="str">
+        <f>VLOOKUP(A73,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Parainfluenza 2</v>
+      </c>
+      <c r="C73" s="1" t="str">
+        <f>VLOOKUP(A73,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B74" s="1" t="str">
+        <f>VLOOKUP(A74,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Parainfluenza 3</v>
+      </c>
+      <c r="C74" s="1" t="str">
+        <f>VLOOKUP(A74,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B75" s="1" t="str">
+        <f>VLOOKUP(A75,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Parainfluenza 4</v>
+      </c>
+      <c r="C75" s="1" t="str">
+        <f>VLOOKUP(A75,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B76" s="1" t="str">
+        <f>VLOOKUP(A76,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Adenovírus</v>
+      </c>
+      <c r="C76" s="1" t="str">
+        <f>VLOOKUP(A76,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B77" s="1" t="str">
+        <f>VLOOKUP(A77,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Metapneumovírus</v>
+      </c>
+      <c r="C77" s="1" t="str">
+        <f>VLOOKUP(A77,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B78" s="1" t="str">
+        <f>VLOOKUP(A78,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Bocavírus</v>
+      </c>
+      <c r="C78" s="1" t="str">
+        <f>VLOOKUP(A78,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B79" s="1" t="str">
+        <f>VLOOKUP(A79,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Rinovírus</v>
+      </c>
+      <c r="C79" s="1" t="str">
+        <f>VLOOKUP(A79,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B80" s="1" t="str">
+        <f>VLOOKUP(A80,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para outro vírus respiratório</v>
+      </c>
+      <c r="C80" s="1" t="str">
+        <f>VLOOKUP(A80,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B81" s="1" t="str">
+        <f>VLOOKUP(A81,Tabela5[#All], 2, FALSE)</f>
+        <v>Diagnóstico final do caso</v>
+      </c>
+      <c r="C81" s="1" t="str">
+        <f>VLOOKUP(A81,Tabela5[#All], 3, FALSE)</f>
+        <v>1-SRAG por influenza
+2-SRAG por outro vírus respiratório
+3-SRAG por outro agente etiológico, qual:
+4-SRAG não especificado
+5-SRAG por covid-19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B82" s="1" t="str">
+        <f>VLOOKUP(A82,Tabela5[#All], 2, FALSE)</f>
+        <v>Critério de confirmação</v>
+      </c>
+      <c r="C82" s="1" t="str">
+        <f>VLOOKUP(A82,Tabela5[#All], 3, FALSE)</f>
+        <v>1. Laboratorial_x000D_
+2. Clínico Epidemiológico_x000D_
+3. Clínico_x000D_
+4. Clínico Imagem</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B83" s="1" t="str">
+        <f>VLOOKUP(A83,Tabela5[#All], 2, FALSE)</f>
+        <v>Evolução do caso</v>
+      </c>
+      <c r="C83" s="1" t="str">
+        <f>VLOOKUP(A83,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Cura
+2-Óbito
+3- Óbito por outras causas
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B84" s="1" t="str">
+        <f>VLOOKUP(A84,Tabela5[#All], 2, FALSE)</f>
+        <v>Histórico de viagem do paciente</v>
+      </c>
+      <c r="C84" s="1" t="str">
+        <f>VLOOKUP(A84,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B85" s="1" t="str">
+        <f>VLOOKUP(A85,Tabela5[#All], 2, FALSE)</f>
+        <v>País de viagem do paciente</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B86" s="1" t="str">
+        <f>VLOOKUP(A86,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para SARS2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B87" s="1" t="str">
+        <f>VLOOKUP(A87,Tabela5[#All], 2, FALSE)</f>
+        <v>Caso contato com outro animal, o mesmo deve ser especificado</v>
+      </c>
+      <c r="C87" s="1" t="str">
+        <f>VLOOKUP(A87,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B88" s="1" t="str">
+        <f>VLOOKUP(A88,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou dor abdominal</v>
+      </c>
+      <c r="C88" s="1" t="str">
+        <f>VLOOKUP(A88,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89" s="1" t="str">
+        <f>VLOOKUP(A89,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou fadiga</v>
+      </c>
+      <c r="C89" s="1" t="str">
+        <f>VLOOKUP(A89,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B90" s="1" t="str">
+        <f>VLOOKUP(A90,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou perda do olfato</v>
+      </c>
+      <c r="C90" s="1" t="str">
+        <f>VLOOKUP(A90,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B91" s="1" t="str">
+        <f>VLOOKUP(A91,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente apresentou perda do paladar</v>
+      </c>
+      <c r="C91" s="1" t="str">
+        <f>VLOOKUP(A91,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B92" s="1" t="str">
+        <f>VLOOKUP(A92,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado da tomografia</v>
+      </c>
+      <c r="C92" s="1" t="str">
+        <f>VLOOKUP(A92,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Tipico covid-19_x000D_
+2- Indeterminado covid-19_x000D_
+3- Atípico covid-19_x000D_
+4- Negativo para Pneumonia_x000D_
+5- Outro_x000D_
+6-Não realizado_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B93" s="1" t="str">
+        <f>VLOOKUP(A93,Tabela5[#All], 2, FALSE)</f>
+        <v>Tipo de teste antigênico</v>
+      </c>
+      <c r="C93" s="1" t="str">
+        <f>VLOOKUP(A93,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Imunofluorescência (IF)_x000D_
+2- Teste rápido antigênico</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B94" s="1" t="str">
+        <f>VLOOKUP(A94,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste antigênico</v>
+      </c>
+      <c r="C94" s="1" t="str">
+        <f>VLOOKUP(A94,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Positivo
+2-Negativo
+3- Inconclusivo
+4-Não realizado
+5-Aguardando resultado
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B95" s="1" t="str">
+        <f>VLOOKUP(A95,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste foi positivo Influenza</v>
+      </c>
+      <c r="C95" s="1" t="str">
+        <f>VLOOKUP(A95,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim_x000D_
+2-Não_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B96" s="1" t="str">
+        <f>VLOOKUP(A96,Tabela5[#All], 2, FALSE)</f>
+        <v>Se influenza, tipo</v>
+      </c>
+      <c r="C96" s="1" t="str">
+        <f>VLOOKUP(A96,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Influenza A
+2-Influenza B</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B97" s="1" t="str">
+        <f>VLOOKUP(A97,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste positivo para outro vírus</v>
+      </c>
+      <c r="C97" s="1" t="str">
+        <f>VLOOKUP(A97,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim_x000D_
+2-Não_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B98" s="1" t="str">
+        <f>VLOOKUP(A98,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste para SARS-CoV-2</v>
+      </c>
+      <c r="C98" s="1" t="str">
+        <f>VLOOKUP(A98,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B99" s="1" t="str">
+        <f>VLOOKUP(A99,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste para VSR</v>
+      </c>
+      <c r="C99" s="1" t="str">
+        <f>VLOOKUP(A99,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B100" s="1" t="str">
+        <f>VLOOKUP(A100,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste para Parainfluenza 1</v>
+      </c>
+      <c r="C100" s="1" t="str">
+        <f>VLOOKUP(A100,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B101" s="1" t="str">
+        <f>VLOOKUP(A101,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste para Parainfluenza 2</v>
+      </c>
+      <c r="C101" s="1" t="str">
+        <f>VLOOKUP(A101,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B102" s="1" t="str">
+        <f>VLOOKUP(A102,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste para Parainfluenza 3</v>
+      </c>
+      <c r="C102" s="1" t="str">
+        <f>VLOOKUP(A102,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B103" s="1" t="str">
+        <f>VLOOKUP(A103,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste para Adenovírus</v>
+      </c>
+      <c r="C103" s="1" t="str">
+        <f>VLOOKUP(A103,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B104" s="1" t="str">
+        <f>VLOOKUP(A104,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado do teste para outro vírus respiratório</v>
+      </c>
+      <c r="C104" s="1" t="str">
+        <f>VLOOKUP(A104,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B105" s="1" t="str">
+        <f>VLOOKUP(A105,Tabela5[#All], 2, FALSE)</f>
+        <v>Nome do outro vírus identificado pelo teste</v>
+      </c>
+      <c r="C105" s="1" t="str">
+        <f>VLOOKUP(A105,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B106" s="1" t="str">
+        <f>VLOOKUP(A106,Tabela5[#All], 2, FALSE)</f>
+        <v>Tipo de amostra sorológica coletada</v>
+      </c>
+      <c r="C106" s="1" t="str">
+        <f>VLOOKUP(A106,Tabela5[#All], 3, FALSE)</f>
+        <v xml:space="preserve">1- Sangue/plasma/soro_x000D_
+2-Outra, qual?_x000D_
+9-Ignorado </v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B107" s="1" t="str">
+        <f>VLOOKUP(A107,Tabela5[#All], 2, FALSE)</f>
+        <v>Tipo do teste sorológico para SARS-CoV-2</v>
+      </c>
+      <c r="C107" s="1" t="str">
+        <f>VLOOKUP(A107,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Teste rápido_x000D_
+2-Elisa_x000D_
+3- Quimiluminescência_x000D_
+4- Outro, qual</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B108" s="1" t="str">
+        <f>VLOOKUP(A108,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado da Sorologia para SARS-CoV-2</v>
+      </c>
+      <c r="C108" s="1" t="str">
+        <f>VLOOKUP(A108,Tabela5[#All], 3, FALSE)</f>
+        <v>IgG (Imunoglobulina G)</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B109" s="1" t="str">
+        <f>VLOOKUP(A109,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado da Sorologia para SARS-CoV-2</v>
+      </c>
+      <c r="C109" s="1" t="str">
+        <f>VLOOKUP(A109,Tabela5[#All], 3, FALSE)</f>
+        <v>IgM (Imunoglobulina M)</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B110" s="1" t="str">
+        <f>VLOOKUP(A110,Tabela5[#All], 2, FALSE)</f>
+        <v>Resultado da Sorologia para SARS-CoV-2</v>
+      </c>
+      <c r="C110" s="1" t="str">
+        <f>VLOOKUP(A110,Tabela5[#All], 3, FALSE)</f>
+        <v>IgA (Imunoglobulina A)</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B111" s="1" t="str">
+        <f>VLOOKUP(A111,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente recebeu a vacina da COVID-19</v>
+      </c>
+      <c r="C111" s="1" t="str">
+        <f>VLOOKUP(A111,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B112" s="1" t="str">
+        <f>VLOOKUP(A112,Tabela5[#All], 2, FALSE)</f>
+        <v>Data que o paciente recebeu a 1a dose</v>
+      </c>
+      <c r="C112" s="1" t="str">
+        <f>VLOOKUP(A112,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B113" s="1" t="str">
+        <f>VLOOKUP(A113,Tabela5[#All], 2, FALSE)</f>
+        <v>Data que o paciente recebeu a 2a dose</v>
+      </c>
+      <c r="C113" s="1" t="str">
+        <f>VLOOKUP(A113,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B114" s="1" t="str">
+        <f>VLOOKUP(A114,Tabela5[#All], 2, FALSE)</f>
+        <v>Data que o paciente recebeu a dose de reforço</v>
+      </c>
+      <c r="C114" s="1" t="str">
+        <f>VLOOKUP(A114,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B115" s="1" t="str">
+        <f>VLOOKUP(A115,Tabela5[#All], 2, FALSE)</f>
+        <v>Fabricante da vacina da 1a dose</v>
+      </c>
+      <c r="C115" s="1" t="str">
+        <f>VLOOKUP(A115,Tabela5[#All], 3, FALSE)</f>
+        <v>Esta com nome FAB_COV1 no dicionário</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B116" s="1" t="str">
+        <f>VLOOKUP(A116,Tabela5[#All], 2, FALSE)</f>
+        <v>Fabricante da vacina da 2a dose</v>
+      </c>
+      <c r="C116" s="1" t="str">
+        <f>VLOOKUP(A116,Tabela5[#All], 3, FALSE)</f>
+        <v>Esta com nome FAB_COV2 no dicionário</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B117" s="1" t="str">
+        <f>VLOOKUP(A117,Tabela5[#All], 2, FALSE)</f>
+        <v>Fabricante da vacina da dose de reforço</v>
+      </c>
+      <c r="C117" s="1" t="str">
+        <f>VLOOKUP(A117,Tabela5[#All], 3, FALSE)</f>
+        <v>Esta com nome FAB_COVRF no dicionário</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B118" s="1" t="str">
+        <f>VLOOKUP(A118,Tabela5[#All], 2, FALSE)</f>
+        <v>Lote da 1a dose da vacina</v>
+      </c>
+      <c r="C118" s="1" t="str">
+        <f>VLOOKUP(A118,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B119" s="1" t="str">
+        <f>VLOOKUP(A119,Tabela5[#All], 2, FALSE)</f>
+        <v>Lote da 2a dose da vacina</v>
+      </c>
+      <c r="C119" s="1" t="str">
+        <f>VLOOKUP(A119,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B120" s="1" t="str">
+        <f>VLOOKUP(A120,Tabela5[#All], 2, FALSE)</f>
+        <v>Lote da dose de reforço da vacina</v>
+      </c>
+      <c r="C120" s="1" t="str">
+        <f>VLOOKUP(A120,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B121" s="1" t="str">
+        <f>VLOOKUP(A121,Tabela5[#All], 2, FALSE)</f>
+        <v>Data que o paciente recebeu a 2a dose de reforço</v>
+      </c>
+      <c r="C121" s="1" t="str">
+        <f>VLOOKUP(A121,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B122" s="1" t="str">
+        <f>VLOOKUP(A122,Tabela5[#All], 2, FALSE)</f>
+        <v>Fabricante da vacina da 2a dose de reforço</v>
+      </c>
+      <c r="C122" s="1" t="str">
+        <f>VLOOKUP(A122,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B123" s="1" t="str">
+        <f>VLOOKUP(A123,Tabela5[#All], 2, FALSE)</f>
+        <v>Lote da 2a dose de reforço da vacina</v>
+      </c>
+      <c r="C123" s="1" t="str">
+        <f>VLOOKUP(A123,Tabela5[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B124" s="1" t="str">
+        <f>VLOOKUP(A124,Tabela5[#All], 2, FALSE)</f>
+        <v>Paciente fez uso de antiviral para tratamento de COVID-19</v>
+      </c>
+      <c r="C124" s="1" t="str">
+        <f>VLOOKUP(A124,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B125" s="1" t="str">
+        <f>VLOOKUP(A125,Tabela5[#All], 2, FALSE)</f>
+        <v>Se TRAT_COV == 1, qual antiviral</v>
+      </c>
+      <c r="C125" s="1" t="str">
+        <f>VLOOKUP(A125,Tabela5[#All], 3, FALSE)</f>
+        <v>1-Nirmatrevir/ritonavir(Paxlovid ®)
+2- Molnupiravir(Lagevrio®)
+3- Baricitinibe (Olumiant®)
+4- Outro, especifique</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1710726D-0BE6-4091-BBA6-4ED458250109}">
+  <dimension ref="A1:C125"/>
+  <sheetViews>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="59" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>VLOOKUP(A2,Tabela6[#All], 2, FALSE)</f>
+        <v>Semana Epidemiológica do preenchimento da ficha de notificação</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>VLOOKUP(A2,Tabela6[#All], 3, FALSE)</f>
+        <v>As Semanas Epidemiológicas (SE) são contadas de um Domingo até o Sábado.
+Se o ano começa em uma segunda-feira, a 1ª SE começará no domingo da mesma semana.</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>VLOOKUP(A3,Tabela6[#All], 2, FALSE)</f>
+        <v>Semana Epidemiológica do início dos sintomas</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>VLOOKUP(A3,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>VLOOKUP(A4,Tabela6[#All], 2, FALSE)</f>
+        <v>Unidade Federativa</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>VLOOKUP(A4,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f>VLOOKUP(A5,Tabela6[#All], 2, FALSE)</f>
+        <v>Regional de Saúde</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f>VLOOKUP(A6,Tabela6[#All], 2, FALSE)</f>
+        <v>Município</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f>VLOOKUP(A7,Tabela6[#All], 2, FALSE)</f>
+        <v>Unidade que realizou o atendimento, coleta de amostra e registro do caso</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f>VLOOKUP(A8,Tabela6[#All], 2, FALSE)</f>
+        <v>Sexo do paciente</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f>VLOOKUP(A8,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Masculino
+2-Feminino
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>VLOOKUP(A9,Tabela6[#All], 2, FALSE)</f>
+        <v>Idade do paciente</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>VLOOKUP(A9,Tabela6[#All], 3, FALSE)</f>
+        <v>Caso tenha sido fornecida a data de nascimento esse campo é preenchido automaticamente (considerando o intervalo entre a data de nascimento e a data dos primeiros sintomas), caso não, é preenchido com a idade informada pelo paciente</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f>VLOOKUP(A10,Tabela6[#All], 2, FALSE)</f>
+        <v>Tipo do campo idade</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>VLOOKUP(A10,Tabela6[#All], 3, FALSE)</f>
+        <v>Se a diferença entre a data de nascimento e a data dos primeiros sintomas for:
+Menor que 1 mês: o tipo é preenchido como 1-Dia
+De 1 a 11 meses: o tipo é preenchido como 2-Mês
+Maior ou igual a 12 meses: o tipo é preenchido como 3-Ano</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>VLOOKUP(A11,Tabela6[#All], 2, FALSE)</f>
+        <v xml:space="preserve">Idade gestacional da paciente.
+</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>VLOOKUP(A11,Tabela6[#All], 3, FALSE)</f>
+        <v>1-1º Trimestre
+2-2º Trimestre
+3-3º Trimestre
+4-Idade Gestacional Ignorada
+5-Não
+6-Não se aplica
+9-Ignorado
+Se selecionado sexo igual a Masculino ou a idade for menor ou igual a 9 anos o campo é preenchido automaticamente com 6-Não se aplica</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f>VLOOKUP(A12,Tabela6[#All], 2, FALSE)</f>
+        <v>Cor ou raça declarada pelo paciente</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>VLOOKUP(A12,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Branca
+2-Preta
+3-Amarela
+4-Parda
+5-Indígena
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f>VLOOKUP(A13,Tabela6[#All], 2, FALSE)</f>
+        <v>Nível de escolaridade do paciente</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>VLOOKUP(A13,Tabela6[#All], 3, FALSE)</f>
+        <v>0-Sem escolaridade/ Analfabeto
+1-Fundamental 1º ciclo (1ª a 5ª série)
+2-Fundamental 2º ciclo (6ª a 9ª série)
+3- Médio (1º ao 3º ano)
+4-Superior
+5-Não se aplica
+9-Ignorado
+Se o paciente tiver menos de 7 anos é automaticamente preenchido com a categoria “não se aplica”</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f>VLOOKUP(A14,Tabela6[#All], 2, FALSE)</f>
+        <v>País de residência do paciente</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f>VLOOKUP(A15,Tabela6[#All], 2, FALSE)</f>
+        <v>UF da residência</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f>VLOOKUP(A16,Tabela6[#All], 2, FALSE)</f>
+        <v>Regional de Saúde onde está localizado o Município de residência do paciente</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f>VLOOKUP(A17,Tabela6[#All], 2, FALSE)</f>
+        <v>Município de residência do paciente</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f>VLOOKUP(A18,Tabela6[#All], 2, FALSE)</f>
+        <v>Zona geográfica da residência</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>VLOOKUP(A18,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Urbana
+2-Rural
+3-Periurbana
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f>VLOOKUP(A19,Tabela6[#All], 2, FALSE)</f>
+        <v>Caso de SRAG com infecção adquirida após internação</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f>VLOOKUP(A19,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f>VLOOKUP(A20,Tabela6[#All], 2, FALSE)</f>
+        <v>Caso com contato direto com aves ou suínos</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>VLOOKUP(A20,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f>VLOOKUP(A21,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou febre</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>VLOOKUP(A21,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f>VLOOKUP(A22,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou tosse</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f>VLOOKUP(A22,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f>VLOOKUP(A23,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou dor de garganta</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f>VLOOKUP(A23,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f>VLOOKUP(A24,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou dispneia</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f>VLOOKUP(A24,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f>VLOOKUP(A25,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou desconforto respiratório</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>VLOOKUP(A25,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f>VLOOKUP(A26,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou saturção O2 &lt; 95%</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f>VLOOKUP(A26,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f>VLOOKUP(A27,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou diarreia</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f>VLOOKUP(A27,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f>VLOOKUP(A28,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou vômito</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <f>VLOOKUP(A28,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <f>VLOOKUP(A29,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou outros sintomas</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <f>VLOOKUP(A29,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <f>VLOOKUP(A30,Tabela6[#All], 2, FALSE)</f>
+        <v>Lista outros sintomas</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <f>VLOOKUP(A30,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <f>VLOOKUP(A31,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente é puérpera ou parturiente (até 45 dias após o parto)</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <f>VLOOKUP(A31,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <f>VLOOKUP(A32,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresenta algum fator de risco</v>
+      </c>
+      <c r="C32" s="1" t="str">
+        <f>VLOOKUP(A32,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <f>VLOOKUP(A33,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui doença cardiovascular crônica</v>
+      </c>
+      <c r="C33" s="1" t="str">
+        <f>VLOOKUP(A33,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <f>VLOOKUP(A34,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui doença hematológica crônica</v>
+      </c>
+      <c r="C34" s="1" t="str">
+        <f>VLOOKUP(A34,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f>VLOOKUP(A35,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui síndrome de down</v>
+      </c>
+      <c r="C35" s="1" t="str">
+        <f>VLOOKUP(A35,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f>VLOOKUP(A36,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui doença hepática crônica</v>
+      </c>
+      <c r="C36" s="1" t="str">
+        <f>VLOOKUP(A36,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f>VLOOKUP(A37,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui asma</v>
+      </c>
+      <c r="C37" s="1" t="str">
+        <f>VLOOKUP(A37,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f>VLOOKUP(A38,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui diabetes mellitus</v>
+      </c>
+      <c r="C38" s="1" t="str">
+        <f>VLOOKUP(A38,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f>VLOOKUP(A39,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui doença neurológica</v>
+      </c>
+      <c r="C39" s="1" t="str">
+        <f>VLOOKUP(A39,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f>VLOOKUP(A40,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui pneumopatia crônica</v>
+      </c>
+      <c r="C40" s="1" t="str">
+        <f>VLOOKUP(A40,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f>VLOOKUP(A41,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui imunodeficiência ou imunodpressão</v>
+      </c>
+      <c r="C41" s="1" t="str">
+        <f>VLOOKUP(A41,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="1" t="str">
+        <f>VLOOKUP(A42,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui doença renal crônica</v>
+      </c>
+      <c r="C42" s="1" t="str">
+        <f>VLOOKUP(A42,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" s="1" t="str">
+        <f>VLOOKUP(A43,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui obesidade</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <f>VLOOKUP(A43,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" s="1" t="str">
+        <f>VLOOKUP(A44,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente possui outro fator de risco</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <f>VLOOKUP(A44,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="1" t="str">
+        <f>VLOOKUP(A45,Tabela6[#All], 2, FALSE)</f>
+        <v>Lista outros fatores de risco do paciente</v>
+      </c>
+      <c r="C45" s="1" t="str">
+        <f>VLOOKUP(A45,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B46" s="1" t="str">
+        <f>VLOOKUP(A46,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente foi vacinado contra a gripe na última campanha</v>
+      </c>
+      <c r="C46" s="1" t="str">
+        <f>VLOOKUP(A46,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B47" s="1" t="str">
+        <f>VLOOKUP(A47,Tabela6[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver menos que 6 meses de vida, a mãe recebeu vacina</v>
+      </c>
+      <c r="C47" s="1" t="str">
+        <f>VLOOKUP(A47,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" s="1" t="str">
+        <f>VLOOKUP(A48,Tabela6[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver menos que 6 meses, a mãe amamenta a criança</v>
+      </c>
+      <c r="C48" s="1" t="str">
+        <f>VLOOKUP(A48,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B49" s="1" t="str">
+        <f>VLOOKUP(A49,Tabela6[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver entre 6 meses e 8 anos, data da dose única para crianças vacinadas em campanhas de anos anteriores</v>
+      </c>
+      <c r="C49" s="1" t="str">
+        <f>VLOOKUP(A49,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B50" s="1" t="str">
+        <f>VLOOKUP(A50,Tabela6[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver entre 6 meses e 8 anos, data da 1a dose para crianças vacinadas pela primeira vez</v>
+      </c>
+      <c r="C50" s="1" t="str">
+        <f>VLOOKUP(A50,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f>VLOOKUP(A51,Tabela6[#All], 2, FALSE)</f>
+        <v>Se o paciente tiver entre 6 meses e 8 anos, data da 2a dose para crianças vacinadas pela primeira vez</v>
+      </c>
+      <c r="C51" s="1" t="str">
+        <f>VLOOKUP(A51,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f>VLOOKUP(A52,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente usou antiviral para gripe</v>
+      </c>
+      <c r="C52" s="1" t="str">
+        <f>VLOOKUP(A52,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f>VLOOKUP(A53,Tabela6[#All], 2, FALSE)</f>
+        <v>Qual antiviral</v>
+      </c>
+      <c r="C53" s="1" t="str">
+        <f>VLOOKUP(A53,Tabela6[#All], 3, FALSE)</f>
+        <v>1- Oseltamivir
+2- Zanamivir
+3- Outro, especifique</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f>VLOOKUP(A54,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente foi internado</v>
+      </c>
+      <c r="C54" s="1" t="str">
+        <f>VLOOKUP(A54,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f>VLOOKUP(A55,Tabela6[#All], 2, FALSE)</f>
+        <v>UF onde o paciente foi internado</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f>VLOOKUP(A56,Tabela6[#All], 2, FALSE)</f>
+        <v>Regional de Saúde onde o paciente foi internado</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f>VLOOKUP(A57,Tabela6[#All], 2, FALSE)</f>
+        <v>Município onde o paciente foi internado</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f>VLOOKUP(A58,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente foi internado na UTI</v>
+      </c>
+      <c r="C58" s="1" t="str">
+        <f>VLOOKUP(A58,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f>VLOOKUP(A59,Tabela6[#All], 2, FALSE)</f>
+        <v>Data de entrada na UTI</v>
+      </c>
+      <c r="C59" s="1" t="str">
+        <f>VLOOKUP(A59,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f>VLOOKUP(A60,Tabela6[#All], 2, FALSE)</f>
+        <v>Data de saída da UTI</v>
+      </c>
+      <c r="C60" s="1" t="str">
+        <f>VLOOKUP(A60,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f>VLOOKUP(A61,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente fez uso de suporte ventilatório</v>
+      </c>
+      <c r="C61" s="1" t="str">
+        <f>VLOOKUP(A61,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim, invasivo
+2-Sim, não invasivo
+3-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f>VLOOKUP(A62,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado Raio-X de tórax</v>
+      </c>
+      <c r="C62" s="1" t="str">
+        <f>VLOOKUP(A62,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Normal_x000D_
+2-Infiltrado intersticial_x000D_
+3-Consolidação_x000D_
+4-Misto_x000D_
+5-Outro_x000D_
+6-Não realizado_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B63" s="1" t="str">
+        <f>VLOOKUP(A63,Tabela6[#All], 2, FALSE)</f>
+        <v>Foi realizado coleta de amostra na realização do teste diagnóstico</v>
+      </c>
+      <c r="C63" s="1" t="str">
+        <f>VLOOKUP(A63,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B64" s="1" t="str">
+        <f>VLOOKUP(A64,Tabela6[#All], 2, FALSE)</f>
+        <v>Tipo da amostra</v>
+      </c>
+      <c r="C64" s="1" t="str">
+        <f>VLOOKUP(A64,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Secreção de Nasoorofaringe_x000D_
+2-Lavado Broco-alveolar_x000D_
+3-Tecido post-mortem_x000D_
+4-Outra, qual?_x000D_
+5-LCR_x000D_
+9-Ignorado_x000D_</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B65" s="1" t="str">
+        <f>VLOOKUP(A65,Tabela6[#All], 2, FALSE)</f>
+        <v>Se for colhida amostra, resultado do teste RT-PCR ou outro método</v>
+      </c>
+      <c r="C65" s="1" t="str">
+        <f>VLOOKUP(A65,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Detectável
+2-Não Detectável
+3-Inconclusivo
+4-Não Realizado
+5-Aguardando Resultado
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B66" s="1" t="str">
+        <f>VLOOKUP(A66,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do RT-PCR foi positivo para influenza</v>
+      </c>
+      <c r="C66" s="1" t="str">
+        <f>VLOOKUP(A66,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim_x000D_
+2-Não_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B67" s="1" t="str">
+        <f>VLOOKUP(A67,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do diagnóstico do RT-PCR para o tipo de influenza</v>
+      </c>
+      <c r="C67" s="1" t="str">
+        <f>VLOOKUP(A67,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Influenza A_x000D_
+2-Influenza B</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B68" s="1" t="str">
+        <f>VLOOKUP(A68,Tabela6[#All], 2, FALSE)</f>
+        <v>Subtipo para Influenza A</v>
+      </c>
+      <c r="C68" s="1" t="str">
+        <f>VLOOKUP(A68,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Influenza A(H1N1)pdm09_x000D_
+2-Influenza A (H3N2)_x000D_
+3-Influenza A não subtipado_x000D_
+4-Influenza A não subtipável_x000D_
+5-Inconclusivo_x000D_
+6-Outro, especifique</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B69" s="1" t="str">
+        <f>VLOOKUP(A69,Tabela6[#All], 2, FALSE)</f>
+        <v>Linhagem da Influenza B</v>
+      </c>
+      <c r="C69" s="1" t="str">
+        <f>VLOOKUP(A69,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Victoria
+2-Yamagatha
+3-Não realizado
+4-Inconclusivo
+5-Outro, especifique:</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B70" s="1" t="str">
+        <f>VLOOKUP(A70,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do RT-PCR foi positivo para outro vírus respiratório</v>
+      </c>
+      <c r="C70" s="1" t="str">
+        <f>VLOOKUP(A70,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B71" s="1" t="str">
+        <f>VLOOKUP(A71,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para VSR</v>
+      </c>
+      <c r="C71" s="1" t="str">
+        <f>VLOOKUP(A71,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="B72" s="1" t="str">
+        <f>VLOOKUP(A72,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Parainfluenza 1</v>
+      </c>
+      <c r="C72" s="1" t="str">
+        <f>VLOOKUP(A72,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B73" s="1" t="str">
+        <f>VLOOKUP(A73,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Parainfluenza 2</v>
+      </c>
+      <c r="C73" s="1" t="str">
+        <f>VLOOKUP(A73,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B74" s="1" t="str">
+        <f>VLOOKUP(A74,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Parainfluenza 3</v>
+      </c>
+      <c r="C74" s="1" t="str">
+        <f>VLOOKUP(A74,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B75" s="1" t="str">
+        <f>VLOOKUP(A75,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Parainfluenza 4</v>
+      </c>
+      <c r="C75" s="1" t="str">
+        <f>VLOOKUP(A75,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B76" s="1" t="str">
+        <f>VLOOKUP(A76,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Adenovírus</v>
+      </c>
+      <c r="C76" s="1" t="str">
+        <f>VLOOKUP(A76,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B77" s="1" t="str">
+        <f>VLOOKUP(A77,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Metapneumovírus</v>
+      </c>
+      <c r="C77" s="1" t="str">
+        <f>VLOOKUP(A77,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B78" s="1" t="str">
+        <f>VLOOKUP(A78,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Bocavírus</v>
+      </c>
+      <c r="C78" s="1" t="str">
+        <f>VLOOKUP(A78,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B79" s="1" t="str">
+        <f>VLOOKUP(A79,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para Rinovírus</v>
+      </c>
+      <c r="C79" s="1" t="str">
+        <f>VLOOKUP(A79,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B80" s="1" t="str">
+        <f>VLOOKUP(A80,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para outro vírus respiratório</v>
+      </c>
+      <c r="C80" s="1" t="str">
+        <f>VLOOKUP(A80,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B81" s="1" t="str">
+        <f>VLOOKUP(A81,Tabela6[#All], 2, FALSE)</f>
+        <v>Diagnóstico final do caso</v>
+      </c>
+      <c r="C81" s="1" t="str">
+        <f>VLOOKUP(A81,Tabela6[#All], 3, FALSE)</f>
+        <v>1-SRAG por influenza
+2-SRAG por outro vírus respiratório
+3-SRAG por outro agente etiológico, qual:
+4-SRAG não especificado
+5-SRAG por covid-19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B82" s="1" t="str">
+        <f>VLOOKUP(A82,Tabela6[#All], 2, FALSE)</f>
+        <v>Critério de confirmação</v>
+      </c>
+      <c r="C82" s="1" t="str">
+        <f>VLOOKUP(A82,Tabela6[#All], 3, FALSE)</f>
+        <v>1. Laboratorial_x000D_
+2. Clínico Epidemiológico_x000D_
+3. Clínico_x000D_
+4. Clínico Imagem</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B83" s="1" t="str">
+        <f>VLOOKUP(A83,Tabela6[#All], 2, FALSE)</f>
+        <v>Evolução do caso</v>
+      </c>
+      <c r="C83" s="1" t="str">
+        <f>VLOOKUP(A83,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Cura
+2-Óbito
+3- Óbito por outras causas
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B84" s="1" t="str">
+        <f>VLOOKUP(A84,Tabela6[#All], 2, FALSE)</f>
+        <v>Histórico de viagem do paciente</v>
+      </c>
+      <c r="C84" s="1" t="str">
+        <f>VLOOKUP(A84,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B85" s="1" t="str">
+        <f>VLOOKUP(A85,Tabela6[#All], 2, FALSE)</f>
+        <v>País de viagem do paciente</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B86" s="1" t="str">
+        <f>VLOOKUP(A86,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado diagnóstico do RT-PCR para SARS2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B87" s="1" t="str">
+        <f>VLOOKUP(A87,Tabela6[#All], 2, FALSE)</f>
+        <v>Caso contato com outro animal, o mesmo deve ser especificado</v>
+      </c>
+      <c r="C87" s="1" t="str">
+        <f>VLOOKUP(A87,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B88" s="1" t="str">
+        <f>VLOOKUP(A88,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou dor abdominal</v>
+      </c>
+      <c r="C88" s="1" t="str">
+        <f>VLOOKUP(A88,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89" s="1" t="str">
+        <f>VLOOKUP(A89,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou fadiga</v>
+      </c>
+      <c r="C89" s="1" t="str">
+        <f>VLOOKUP(A89,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B90" s="1" t="str">
+        <f>VLOOKUP(A90,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou perda do olfato</v>
+      </c>
+      <c r="C90" s="1" t="str">
+        <f>VLOOKUP(A90,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B91" s="1" t="str">
+        <f>VLOOKUP(A91,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente apresentou perda do paladar</v>
+      </c>
+      <c r="C91" s="1" t="str">
+        <f>VLOOKUP(A91,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B92" s="1" t="str">
+        <f>VLOOKUP(A92,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado da tomografia</v>
+      </c>
+      <c r="C92" s="1" t="str">
+        <f>VLOOKUP(A92,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Tipico covid-19_x000D_
+2- Indeterminado covid-19_x000D_
+3- Atípico covid-19_x000D_
+4- Negativo para Pneumonia_x000D_
+5- Outro_x000D_
+6-Não realizado_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B93" s="1" t="str">
+        <f>VLOOKUP(A93,Tabela6[#All], 2, FALSE)</f>
+        <v>Tipo de teste antigênico</v>
+      </c>
+      <c r="C93" s="1" t="str">
+        <f>VLOOKUP(A93,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Imunofluorescência (IF)_x000D_
+2- Teste rápido antigênico</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B94" s="1" t="str">
+        <f>VLOOKUP(A94,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste antigênico</v>
+      </c>
+      <c r="C94" s="1" t="str">
+        <f>VLOOKUP(A94,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Positivo
+2-Negativo
+3- Inconclusivo
+4-Não realizado
+5-Aguardando resultado
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B95" s="1" t="str">
+        <f>VLOOKUP(A95,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste foi positivo Influenza</v>
+      </c>
+      <c r="C95" s="1" t="str">
+        <f>VLOOKUP(A95,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim_x000D_
+2-Não_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B96" s="1" t="str">
+        <f>VLOOKUP(A96,Tabela6[#All], 2, FALSE)</f>
+        <v>Se influenza, tipo</v>
+      </c>
+      <c r="C96" s="1" t="str">
+        <f>VLOOKUP(A96,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Influenza A
+2-Influenza B</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B97" s="1" t="str">
+        <f>VLOOKUP(A97,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste positivo para outro vírus</v>
+      </c>
+      <c r="C97" s="1" t="str">
+        <f>VLOOKUP(A97,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim_x000D_
+2-Não_x000D_
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B98" s="1" t="str">
+        <f>VLOOKUP(A98,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste para SARS-CoV-2</v>
+      </c>
+      <c r="C98" s="1" t="str">
+        <f>VLOOKUP(A98,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B99" s="1" t="str">
+        <f>VLOOKUP(A99,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste para VSR</v>
+      </c>
+      <c r="C99" s="1" t="str">
+        <f>VLOOKUP(A99,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B100" s="1" t="str">
+        <f>VLOOKUP(A100,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste para Parainfluenza 1</v>
+      </c>
+      <c r="C100" s="1" t="str">
+        <f>VLOOKUP(A100,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B101" s="1" t="str">
+        <f>VLOOKUP(A101,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste para Parainfluenza 2</v>
+      </c>
+      <c r="C101" s="1" t="str">
+        <f>VLOOKUP(A101,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B102" s="1" t="str">
+        <f>VLOOKUP(A102,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste para Parainfluenza 3</v>
+      </c>
+      <c r="C102" s="1" t="str">
+        <f>VLOOKUP(A102,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B103" s="1" t="str">
+        <f>VLOOKUP(A103,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste para Adenovírus</v>
+      </c>
+      <c r="C103" s="1" t="str">
+        <f>VLOOKUP(A103,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B104" s="1" t="str">
+        <f>VLOOKUP(A104,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado do teste para outro vírus respiratório</v>
+      </c>
+      <c r="C104" s="1" t="str">
+        <f>VLOOKUP(A104,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B105" s="1" t="str">
+        <f>VLOOKUP(A105,Tabela6[#All], 2, FALSE)</f>
+        <v>Nome do outro vírus identificado pelo teste</v>
+      </c>
+      <c r="C105" s="1" t="str">
+        <f>VLOOKUP(A105,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B106" s="1" t="str">
+        <f>VLOOKUP(A106,Tabela6[#All], 2, FALSE)</f>
+        <v>Tipo de amostra sorológica coletada</v>
+      </c>
+      <c r="C106" s="1" t="str">
+        <f>VLOOKUP(A106,Tabela6[#All], 3, FALSE)</f>
+        <v xml:space="preserve">1- Sangue/plasma/soro_x000D_
+2-Outra, qual?_x000D_
+9-Ignorado </v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B107" s="1" t="str">
+        <f>VLOOKUP(A107,Tabela6[#All], 2, FALSE)</f>
+        <v>Tipo do teste sorológico para SARS-CoV-2</v>
+      </c>
+      <c r="C107" s="1" t="str">
+        <f>VLOOKUP(A107,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Teste rápido_x000D_
+2-Elisa_x000D_
+3- Quimiluminescência_x000D_
+4- Outro, qual</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B108" s="1" t="str">
+        <f>VLOOKUP(A108,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado da Sorologia para SARS-CoV-2</v>
+      </c>
+      <c r="C108" s="1" t="str">
+        <f>VLOOKUP(A108,Tabela6[#All], 3, FALSE)</f>
+        <v>IgG (Imunoglobulina G)</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B109" s="1" t="str">
+        <f>VLOOKUP(A109,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado da Sorologia para SARS-CoV-2</v>
+      </c>
+      <c r="C109" s="1" t="str">
+        <f>VLOOKUP(A109,Tabela6[#All], 3, FALSE)</f>
+        <v>IgM (Imunoglobulina M)</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B110" s="1" t="str">
+        <f>VLOOKUP(A110,Tabela6[#All], 2, FALSE)</f>
+        <v>Resultado da Sorologia para SARS-CoV-2</v>
+      </c>
+      <c r="C110" s="1" t="str">
+        <f>VLOOKUP(A110,Tabela6[#All], 3, FALSE)</f>
+        <v>IgA (Imunoglobulina A)</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B111" s="1" t="str">
+        <f>VLOOKUP(A111,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente recebeu a vacina da COVID-19</v>
+      </c>
+      <c r="C111" s="1" t="str">
+        <f>VLOOKUP(A111,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B112" s="1" t="str">
+        <f>VLOOKUP(A112,Tabela6[#All], 2, FALSE)</f>
+        <v>Data que o paciente recebeu a 1a dose</v>
+      </c>
+      <c r="C112" s="1" t="str">
+        <f>VLOOKUP(A112,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B113" s="1" t="str">
+        <f>VLOOKUP(A113,Tabela6[#All], 2, FALSE)</f>
+        <v>Data que o paciente recebeu a 2a dose</v>
+      </c>
+      <c r="C113" s="1" t="str">
+        <f>VLOOKUP(A113,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B114" s="1" t="str">
+        <f>VLOOKUP(A114,Tabela6[#All], 2, FALSE)</f>
+        <v>Data que o paciente recebeu a dose de reforço</v>
+      </c>
+      <c r="C114" s="1" t="str">
+        <f>VLOOKUP(A114,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B115" s="1" t="str">
+        <f>VLOOKUP(A115,Tabela6[#All], 2, FALSE)</f>
+        <v>Fabricante da vacina da 1a dose</v>
+      </c>
+      <c r="C115" s="1" t="str">
+        <f>VLOOKUP(A115,Tabela6[#All], 3, FALSE)</f>
+        <v>Esta com nome FAB_COV1 no dicionário</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B116" s="1" t="str">
+        <f>VLOOKUP(A116,Tabela6[#All], 2, FALSE)</f>
+        <v>Fabricante da vacina da 2a dose</v>
+      </c>
+      <c r="C116" s="1" t="str">
+        <f>VLOOKUP(A116,Tabela6[#All], 3, FALSE)</f>
+        <v>Esta com nome FAB_COV2 no dicionário</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B117" s="1" t="str">
+        <f>VLOOKUP(A117,Tabela6[#All], 2, FALSE)</f>
+        <v>Fabricante da vacina da dose de reforço</v>
+      </c>
+      <c r="C117" s="1" t="str">
+        <f>VLOOKUP(A117,Tabela6[#All], 3, FALSE)</f>
+        <v>Esta com nome FAB_COVRF no dicionário</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B118" s="1" t="str">
+        <f>VLOOKUP(A118,Tabela6[#All], 2, FALSE)</f>
+        <v>Lote da 1a dose da vacina</v>
+      </c>
+      <c r="C118" s="1" t="str">
+        <f>VLOOKUP(A118,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B119" s="1" t="str">
+        <f>VLOOKUP(A119,Tabela6[#All], 2, FALSE)</f>
+        <v>Lote da 2a dose da vacina</v>
+      </c>
+      <c r="C119" s="1" t="str">
+        <f>VLOOKUP(A119,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B120" s="1" t="str">
+        <f>VLOOKUP(A120,Tabela6[#All], 2, FALSE)</f>
+        <v>Lote da dose de reforço da vacina</v>
+      </c>
+      <c r="C120" s="1" t="str">
+        <f>VLOOKUP(A120,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B121" s="1" t="str">
+        <f>VLOOKUP(A121,Tabela6[#All], 2, FALSE)</f>
+        <v>Data que o paciente recebeu a 2a dose de reforço</v>
+      </c>
+      <c r="C121" s="1" t="str">
+        <f>VLOOKUP(A121,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B122" s="1" t="str">
+        <f>VLOOKUP(A122,Tabela6[#All], 2, FALSE)</f>
+        <v>Fabricante da vacina da 2a dose de reforço</v>
+      </c>
+      <c r="C122" s="1" t="str">
+        <f>VLOOKUP(A122,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B123" s="1" t="str">
+        <f>VLOOKUP(A123,Tabela6[#All], 2, FALSE)</f>
+        <v>Lote da 2a dose de reforço da vacina</v>
+      </c>
+      <c r="C123" s="1" t="str">
+        <f>VLOOKUP(A123,Tabela6[#All], 3, FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B124" s="1" t="str">
+        <f>VLOOKUP(A124,Tabela6[#All], 2, FALSE)</f>
+        <v>Paciente fez uso de antiviral para tratamento de COVID-19</v>
+      </c>
+      <c r="C124" s="1" t="str">
+        <f>VLOOKUP(A124,Tabela6[#All], 3, FALSE)</f>
+        <v>1-Sim
+2-Não
+9-Ignorado</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B125" s="1" t="str">
+        <f>VLOOKUP(A125,Tabela6[#All], 2, FALSE)</f>
+        <v>Se TRAT_COV == 1, qual antiviral</v>
+      </c>
+      <c r="C125" s="1" t="str">
+        <f>VLOOKUP(A125,Tabela6[#All], 3, FALSE)</f>
         <v>1-Nirmatrevir/ritonavir(Paxlovid ®)
 2- Molnupiravir(Lagevrio®)
 3- Baricitinibe (Olumiant®)

</xml_diff>